<commit_message>
Pruebas Fuentes de pago SGCM
</commit_message>
<xml_diff>
--- a/SGCM/ENTREGABLES/Configuración/Matriz de Pruebas Configuraciones.xlsx
+++ b/SGCM/ENTREGABLES/Configuración/Matriz de Pruebas Configuraciones.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="113">
   <si>
     <t>Ambiente QA</t>
   </si>
@@ -446,6 +446,57 @@
   </si>
   <si>
     <t>https://srpu.atlassian.net/browse/SGCM-492</t>
+  </si>
+  <si>
+    <t>Se guardo un nuevo elemento,  se genera en la pantalla principal , arroja mensaje de confirmación exitoso.  ¿Es Elemento o descripción ? ya que al agregar un nuevo elemento dice " Nuevo elemento" Pero en mensaje de Confirmación dice Descripción</t>
+  </si>
+  <si>
+    <t>Ajustar el color del botón Eliminar 
+Ajustar color en botón ok</t>
+  </si>
+  <si>
+    <t>Ajustar el color del botón Editar 
+Ajustar color en botón ok</t>
+  </si>
+  <si>
+    <t>https://srpu.atlassian.net/browse/SGCM-493</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ajustar el mensaje de alerta cuando </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se agrega información en los campos y das clic en botón aceptar</t>
+    </r>
+  </si>
+  <si>
+    <t>Ajustar el color del botón Eliminar
+Ajustar color en botón ok</t>
+  </si>
+  <si>
+    <t>Ajustar el color del botón editar / justar color en botón ok
+Ajustar el mensaje de alerta cuando no se agrega información en los campos y das clic en botón aceptar</t>
+  </si>
+  <si>
+    <t>https://srpu.atlassian.net/browse/SGCM-494</t>
   </si>
 </sst>
 </file>
@@ -805,6 +856,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,15 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -9602,8 +9653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27:N31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9624,94 +9675,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="29" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -9953,16 +10004,16 @@
       <c r="A13" s="21">
         <v>7</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -9981,10 +10032,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="41"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="3" t="s">
         <v>27</v>
       </c>
@@ -10012,10 +10063,10 @@
     </row>
     <row r="15" spans="1:14" ht="132" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="3" t="s">
         <v>28</v>
       </c>
@@ -10043,10 +10094,10 @@
     </row>
     <row r="16" spans="1:14" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="3" t="s">
         <v>29</v>
       </c>
@@ -10074,10 +10125,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="3" t="s">
         <v>30</v>
       </c>
@@ -10099,16 +10150,16 @@
       <c r="A18" s="21">
         <v>8</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -10130,10 +10181,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="3" t="s">
         <v>27</v>
       </c>
@@ -10150,10 +10201,10 @@
     </row>
     <row r="20" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="41"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="3" t="s">
         <v>28</v>
       </c>
@@ -10182,10 +10233,10 @@
     </row>
     <row r="21" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="41"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="3" t="s">
         <v>29</v>
       </c>
@@ -10213,10 +10264,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="3" t="s">
         <v>30</v>
       </c>
@@ -10234,16 +10285,16 @@
       <c r="A23" s="21">
         <v>9</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -10261,10 +10312,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="41"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="3" t="s">
         <v>27</v>
       </c>
@@ -10292,10 +10343,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="41"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="3" t="s">
         <v>28</v>
       </c>
@@ -10323,10 +10374,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="41"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="3" t="s">
         <v>29</v>
       </c>
@@ -10354,10 +10405,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="41"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="3" t="s">
         <v>30</v>
       </c>
@@ -10375,16 +10426,16 @@
       <c r="A28" s="21">
         <v>10</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -10402,10 +10453,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="41"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="3" t="s">
         <v>27</v>
       </c>
@@ -10417,6 +10468,12 @@
       </c>
       <c r="I29" t="s">
         <v>80</v>
+      </c>
+      <c r="K29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L29" t="s">
+        <v>36</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>104</v>
@@ -10427,10 +10484,10 @@
     </row>
     <row r="30" spans="1:14" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="41"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="3" t="s">
         <v>28</v>
       </c>
@@ -10442,6 +10499,12 @@
       </c>
       <c r="I30" t="s">
         <v>81</v>
+      </c>
+      <c r="K30" t="s">
+        <v>46</v>
+      </c>
+      <c r="L30" t="s">
+        <v>36</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>104</v>
@@ -10452,10 +10515,10 @@
     </row>
     <row r="31" spans="1:14" ht="231" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="41"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="3" t="s">
         <v>29</v>
       </c>
@@ -10477,10 +10540,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="41"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="3" t="s">
         <v>30</v>
       </c>
@@ -10491,170 +10554,290 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
         <v>11</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
       <c r="I33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="41"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
       <c r="I34" t="s">
         <v>80</v>
       </c>
+      <c r="K34" t="s">
+        <v>46</v>
+      </c>
+      <c r="L34" t="s">
+        <v>36</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N34" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="41"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="I35" t="s">
         <v>81</v>
       </c>
+      <c r="K35" t="s">
+        <v>46</v>
+      </c>
+      <c r="L35" t="s">
+        <v>36</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N35" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" s="21"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="41"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="G36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="I36" t="s">
         <v>82</v>
       </c>
+      <c r="K36" t="s">
+        <v>46</v>
+      </c>
+      <c r="L36" t="s">
+        <v>36</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N36" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="21"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="41"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
       <c r="I37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
         <v>12</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
       <c r="I38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="21"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="41"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
       <c r="F39" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="G39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" t="s">
+        <v>109</v>
+      </c>
       <c r="I39" t="s">
         <v>80</v>
       </c>
+      <c r="K39" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" t="s">
+        <v>36</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N39" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="41"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
       <c r="F40" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="G40" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="I40" t="s">
         <v>81</v>
       </c>
+      <c r="K40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" t="s">
+        <v>36</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N40" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="41"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
       <c r="F41" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="G41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="I41" t="s">
         <v>82</v>
       </c>
+      <c r="K41" t="s">
+        <v>46</v>
+      </c>
+      <c r="L41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N41" s="1">
+        <v>45128</v>
+      </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="21"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="41"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
       <c r="F42" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
       <c r="I42" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="21">
         <v>13</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="41" t="s">
+      <c r="E43" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -10664,12 +10847,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="41"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
       <c r="F44" s="3" t="s">
         <v>27</v>
       </c>
@@ -10677,12 +10860,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="41"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
       <c r="F45" s="3" t="s">
         <v>28</v>
       </c>
@@ -10690,12 +10873,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="21"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="41"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
       <c r="F46" s="3" t="s">
         <v>29</v>
       </c>
@@ -10703,12 +10886,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="21"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="41"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
       <c r="F47" s="3" t="s">
         <v>30</v>
       </c>
@@ -10716,20 +10899,20 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="21">
         <v>14</v>
       </c>
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D48" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -10741,10 +10924,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="21"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="41"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
       <c r="F49" s="3" t="s">
         <v>27</v>
       </c>
@@ -10754,10 +10937,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="21"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="41"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
       <c r="F50" s="3" t="s">
         <v>28</v>
       </c>
@@ -10767,10 +10950,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="21"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="41"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
       <c r="F51" s="3" t="s">
         <v>29</v>
       </c>
@@ -10780,10 +10963,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="21"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="41"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="24"/>
       <c r="F52" s="3" t="s">
         <v>30</v>
       </c>
@@ -10795,16 +10978,16 @@
       <c r="A53" s="21">
         <v>15</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F53" s="3" t="s">
@@ -10816,10 +10999,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="21"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="41"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
       <c r="F54" s="3" t="s">
         <v>27</v>
       </c>
@@ -10829,10 +11012,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="41"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
       <c r="F55" s="3" t="s">
         <v>28</v>
       </c>
@@ -10842,10 +11025,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="21"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="41"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
       <c r="F56" s="3" t="s">
         <v>29</v>
       </c>
@@ -10855,10 +11038,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="21"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="41"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="24"/>
       <c r="F57" s="3" t="s">
         <v>30</v>
       </c>
@@ -10870,16 +11053,16 @@
       <c r="A58" s="21">
         <v>16</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D58" s="39" t="s">
+      <c r="D58" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="41" t="s">
+      <c r="E58" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -10891,10 +11074,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="21"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="41"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
       <c r="F59" s="3" t="s">
         <v>27</v>
       </c>
@@ -10904,10 +11087,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="21"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="41"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
       <c r="F60" s="3" t="s">
         <v>28</v>
       </c>
@@ -10917,10 +11100,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="21"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="41"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
       <c r="F61" s="3" t="s">
         <v>29</v>
       </c>
@@ -10930,10 +11113,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="21"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="41"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="24"/>
       <c r="F62" s="3" t="s">
         <v>30</v>
       </c>
@@ -10945,16 +11128,16 @@
       <c r="A63" s="21">
         <v>17</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="39" t="s">
+      <c r="D63" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E63" s="41" t="s">
+      <c r="E63" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -10966,10 +11149,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="21"/>
-      <c r="B64" s="40"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="41"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="24"/>
       <c r="F64" s="3" t="s">
         <v>27</v>
       </c>
@@ -10979,10 +11162,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="21"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="41"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="24"/>
       <c r="F65" s="3" t="s">
         <v>28</v>
       </c>
@@ -10992,10 +11175,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="21"/>
-      <c r="B66" s="40"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="41"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="24"/>
       <c r="F66" s="3" t="s">
         <v>29</v>
       </c>
@@ -11005,10 +11188,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="21"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="41"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="24"/>
       <c r="F67" s="3" t="s">
         <v>30</v>
       </c>
@@ -11020,16 +11203,16 @@
       <c r="A68" s="21">
         <v>18</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="39" t="s">
+      <c r="C68" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="39" t="s">
+      <c r="D68" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E68" s="41" t="s">
+      <c r="E68" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -11041,10 +11224,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="21"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="41"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24"/>
       <c r="F69" s="3" t="s">
         <v>27</v>
       </c>
@@ -11054,10 +11237,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="21"/>
-      <c r="B70" s="40"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="41"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="24"/>
       <c r="F70" s="3" t="s">
         <v>28</v>
       </c>
@@ -11067,10 +11250,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="21"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="41"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="24"/>
       <c r="F71" s="3" t="s">
         <v>29</v>
       </c>
@@ -11080,10 +11263,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="21"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="41"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24"/>
       <c r="F72" s="3" t="s">
         <v>30</v>
       </c>
@@ -11095,16 +11278,16 @@
       <c r="A73" s="21">
         <v>19</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="39" t="s">
+      <c r="C73" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D73" s="39" t="s">
+      <c r="D73" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E73" s="41" t="s">
+      <c r="E73" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -11116,10 +11299,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="21"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="41"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="24"/>
       <c r="F74" s="3" t="s">
         <v>27</v>
       </c>
@@ -11129,10 +11312,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="21"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="41"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
       <c r="F75" s="3" t="s">
         <v>28</v>
       </c>
@@ -11142,10 +11325,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="21"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="41"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="24"/>
       <c r="F76" s="3" t="s">
         <v>29</v>
       </c>
@@ -11155,10 +11338,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="21"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="41"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="24"/>
       <c r="F77" s="3" t="s">
         <v>30</v>
       </c>
@@ -11170,16 +11353,16 @@
       <c r="A78" s="21">
         <v>20</v>
       </c>
-      <c r="B78" s="40" t="s">
+      <c r="B78" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="C78" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D78" s="39" t="s">
+      <c r="D78" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E78" s="41" t="s">
+      <c r="E78" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -11191,10 +11374,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="21"/>
-      <c r="B79" s="40"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="41"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24"/>
       <c r="F79" s="3" t="s">
         <v>27</v>
       </c>
@@ -11204,10 +11387,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="21"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="41"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="24"/>
       <c r="F80" s="3" t="s">
         <v>28</v>
       </c>
@@ -11217,10 +11400,10 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="21"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="41"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
       <c r="F81" s="3" t="s">
         <v>29</v>
       </c>
@@ -11230,10 +11413,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="21"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="41"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="24"/>
       <c r="F82" s="3" t="s">
         <v>30</v>
       </c>
@@ -11245,16 +11428,16 @@
       <c r="A83" s="21">
         <v>21</v>
       </c>
-      <c r="B83" s="40" t="s">
+      <c r="B83" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C83" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D83" s="39" t="s">
+      <c r="D83" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E83" s="41" t="s">
+      <c r="E83" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F83" s="3" t="s">
@@ -11266,10 +11449,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="21"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="41"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="24"/>
       <c r="F84" s="3" t="s">
         <v>27</v>
       </c>
@@ -11279,10 +11462,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
-      <c r="B85" s="40"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="41"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="24"/>
       <c r="F85" s="3" t="s">
         <v>28</v>
       </c>
@@ -11292,10 +11475,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="21"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="41"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="24"/>
       <c r="F86" s="3" t="s">
         <v>29</v>
       </c>
@@ -11305,10 +11488,10 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="21"/>
-      <c r="B87" s="40"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="41"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="24"/>
       <c r="F87" s="3" t="s">
         <v>30</v>
       </c>
@@ -11333,66 +11516,18 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="82">
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="D73:D77"/>
-    <mergeCell ref="E73:E77"/>
-    <mergeCell ref="A68:A72"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="C68:C72"/>
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="B63:B67"/>
-    <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D63:D67"/>
-    <mergeCell ref="E63:E67"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="D58:D62"/>
-    <mergeCell ref="E58:E62"/>
-    <mergeCell ref="A58:A62"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="D53:D57"/>
-    <mergeCell ref="E53:E57"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="E48:E52"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="E38:E42"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="E33:E37"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
-    <mergeCell ref="E28:E32"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:N5"/>
     <mergeCell ref="C18:C22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A18:A22"/>
@@ -11401,20 +11536,68 @@
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="A13:A17"/>
     <mergeCell ref="D18:D22"/>
     <mergeCell ref="E18:E22"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="D28:D32"/>
+    <mergeCell ref="E28:E32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="E33:E37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="E38:E42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="C48:C52"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="E48:E52"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="D53:D57"/>
+    <mergeCell ref="E53:E57"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="D58:D62"/>
+    <mergeCell ref="E58:E62"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D63:D67"/>
+    <mergeCell ref="E63:E67"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="D68:D72"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="A73:A77"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="D73:D77"/>
+    <mergeCell ref="E73:E77"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="E83:E87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
@@ -11425,9 +11608,13 @@
     <hyperlink ref="M25:M26" r:id="rId6" display="https://srpu.atlassian.net/browse/SGCM-489"/>
     <hyperlink ref="M29" r:id="rId7"/>
     <hyperlink ref="M30:M31" r:id="rId8" display="https://srpu.atlassian.net/browse/SGCM-492"/>
+    <hyperlink ref="M34" r:id="rId9"/>
+    <hyperlink ref="M35:M36" r:id="rId10" display="https://srpu.atlassian.net/browse/SGCM-493"/>
+    <hyperlink ref="M39" r:id="rId11"/>
+    <hyperlink ref="M40:M41" r:id="rId12" display="https://srpu.atlassian.net/browse/SGCM-494"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -11441,13 +11628,13 @@
           <x14:formula1>
             <xm:f>Datos!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L8:L21 L24:L26</xm:sqref>
+          <xm:sqref>L8:L21 L24:L26 L29:L30 L34:L36 L39:L41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>K7:K21 K24:K26</xm:sqref>
+          <xm:sqref>K7:K21 K24:K26 K29:K30 K34:K36 K39:K41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>